<commit_message>
For mercycorps/TolaActivity#2539, update alignments and number formats.
</commit_message>
<xml_diff>
--- a/indicators/bulk_import_files/BulkIndicatorImportTemplate.xlsx
+++ b/indicators/bulk_import_files/BulkIndicatorImportTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sjogdeo/Sites/tolaActivity/TolaActivity/indicators/bulk_import_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B85A5E4-3ED3-7345-BF39-DB39C19F0312}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE6391DC-6F14-224F-AA09-D10A541F8896}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Import indicators" sheetId="1" r:id="rId1"/>
@@ -404,7 +404,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -547,6 +547,34 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -769,8 +797,8 @@
   <dimension ref="A1:AJ933"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
+      <pane ySplit="6" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -779,7 +807,9 @@
     <col min="2" max="2" width="15.83203125" style="9" customWidth="1"/>
     <col min="3" max="3" width="7.6640625" style="9" customWidth="1"/>
     <col min="4" max="4" width="50.83203125" style="9" customWidth="1"/>
-    <col min="5" max="23" width="30.83203125" style="9" customWidth="1"/>
+    <col min="5" max="11" width="30.83203125" style="9" customWidth="1"/>
+    <col min="12" max="12" width="30.83203125" style="46" customWidth="1"/>
+    <col min="13" max="23" width="30.83203125" style="9" customWidth="1"/>
     <col min="24" max="36" width="7.6640625" style="9" customWidth="1"/>
     <col min="37" max="16384" width="12.6640625" style="9"/>
   </cols>
@@ -798,7 +828,7 @@
       <c r="I1" s="6"/>
       <c r="J1" s="7"/>
       <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
+      <c r="L1" s="40"/>
       <c r="M1" s="7"/>
       <c r="N1" s="7"/>
       <c r="O1" s="6"/>
@@ -838,7 +868,7 @@
       <c r="I2" s="6"/>
       <c r="J2" s="7"/>
       <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
+      <c r="L2" s="40"/>
       <c r="M2" s="7"/>
       <c r="N2" s="7"/>
       <c r="O2" s="6"/>
@@ -876,7 +906,7 @@
       <c r="I3" s="6"/>
       <c r="J3" s="7"/>
       <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
+      <c r="L3" s="40"/>
       <c r="M3" s="7"/>
       <c r="N3" s="7"/>
       <c r="O3" s="6"/>
@@ -916,7 +946,7 @@
       <c r="I4" s="13"/>
       <c r="J4" s="13"/>
       <c r="K4" s="13"/>
-      <c r="L4" s="13"/>
+      <c r="L4" s="41"/>
       <c r="M4" s="13"/>
       <c r="N4" s="14"/>
       <c r="O4" s="15"/>
@@ -956,7 +986,7 @@
       <c r="I5" s="6"/>
       <c r="J5" s="7"/>
       <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
+      <c r="L5" s="40"/>
       <c r="M5" s="7"/>
       <c r="N5" s="7"/>
       <c r="O5" s="6"/>
@@ -1014,7 +1044,7 @@
       <c r="K6" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="L6" s="20" t="s">
+      <c r="L6" s="42" t="s">
         <v>14</v>
       </c>
       <c r="M6" s="22" t="s">
@@ -1076,7 +1106,7 @@
       <c r="I7" s="26"/>
       <c r="J7" s="26"/>
       <c r="K7" s="26"/>
-      <c r="L7" s="26"/>
+      <c r="L7" s="43"/>
       <c r="M7" s="26"/>
       <c r="N7" s="26"/>
       <c r="O7" s="26"/>
@@ -1114,7 +1144,7 @@
       <c r="I8" s="31"/>
       <c r="J8" s="32"/>
       <c r="K8" s="31"/>
-      <c r="L8" s="31"/>
+      <c r="L8" s="44"/>
       <c r="M8" s="32"/>
       <c r="N8" s="32"/>
       <c r="O8" s="31"/>
@@ -1152,7 +1182,7 @@
       <c r="I9" s="31"/>
       <c r="J9" s="32"/>
       <c r="K9" s="31"/>
-      <c r="L9" s="31"/>
+      <c r="L9" s="44"/>
       <c r="M9" s="32"/>
       <c r="N9" s="32"/>
       <c r="O9" s="31"/>
@@ -1190,7 +1220,7 @@
       <c r="I10" s="31"/>
       <c r="J10" s="32"/>
       <c r="K10" s="31"/>
-      <c r="L10" s="31"/>
+      <c r="L10" s="44"/>
       <c r="M10" s="32"/>
       <c r="N10" s="32"/>
       <c r="O10" s="31"/>
@@ -1228,7 +1258,7 @@
       <c r="I11" s="31"/>
       <c r="J11" s="32"/>
       <c r="K11" s="31"/>
-      <c r="L11" s="31"/>
+      <c r="L11" s="44"/>
       <c r="M11" s="32"/>
       <c r="N11" s="32"/>
       <c r="O11" s="31"/>
@@ -1266,7 +1296,7 @@
       <c r="I12" s="31"/>
       <c r="J12" s="32"/>
       <c r="K12" s="31"/>
-      <c r="L12" s="31"/>
+      <c r="L12" s="44"/>
       <c r="M12" s="32"/>
       <c r="N12" s="32"/>
       <c r="O12" s="31"/>
@@ -1304,7 +1334,7 @@
       <c r="I13" s="31"/>
       <c r="J13" s="32"/>
       <c r="K13" s="31"/>
-      <c r="L13" s="31"/>
+      <c r="L13" s="44"/>
       <c r="M13" s="32"/>
       <c r="N13" s="32"/>
       <c r="O13" s="31"/>
@@ -1342,7 +1372,7 @@
       <c r="I14" s="31"/>
       <c r="J14" s="32"/>
       <c r="K14" s="31"/>
-      <c r="L14" s="31"/>
+      <c r="L14" s="44"/>
       <c r="M14" s="32"/>
       <c r="N14" s="32"/>
       <c r="O14" s="31"/>
@@ -1380,7 +1410,7 @@
       <c r="I15" s="31"/>
       <c r="J15" s="32"/>
       <c r="K15" s="31"/>
-      <c r="L15" s="31"/>
+      <c r="L15" s="44"/>
       <c r="M15" s="32"/>
       <c r="N15" s="32"/>
       <c r="O15" s="31"/>
@@ -1418,7 +1448,7 @@
       <c r="I16" s="31"/>
       <c r="J16" s="32"/>
       <c r="K16" s="31"/>
-      <c r="L16" s="31"/>
+      <c r="L16" s="44"/>
       <c r="M16" s="32"/>
       <c r="N16" s="32"/>
       <c r="O16" s="31"/>
@@ -1456,7 +1486,7 @@
       <c r="I17" s="31"/>
       <c r="J17" s="32"/>
       <c r="K17" s="31"/>
-      <c r="L17" s="31"/>
+      <c r="L17" s="44"/>
       <c r="M17" s="32"/>
       <c r="N17" s="32"/>
       <c r="O17" s="31"/>
@@ -1494,7 +1524,7 @@
       <c r="I18" s="31"/>
       <c r="J18" s="32"/>
       <c r="K18" s="31"/>
-      <c r="L18" s="31"/>
+      <c r="L18" s="44"/>
       <c r="M18" s="32"/>
       <c r="N18" s="32"/>
       <c r="O18" s="31"/>
@@ -1532,7 +1562,7 @@
       <c r="I19" s="31"/>
       <c r="J19" s="32"/>
       <c r="K19" s="31"/>
-      <c r="L19" s="31"/>
+      <c r="L19" s="44"/>
       <c r="M19" s="32"/>
       <c r="N19" s="32"/>
       <c r="O19" s="31"/>
@@ -1570,7 +1600,7 @@
       <c r="I20" s="31"/>
       <c r="J20" s="32"/>
       <c r="K20" s="31"/>
-      <c r="L20" s="31"/>
+      <c r="L20" s="44"/>
       <c r="M20" s="32"/>
       <c r="N20" s="32"/>
       <c r="O20" s="31"/>
@@ -1608,7 +1638,7 @@
       <c r="I21" s="31"/>
       <c r="J21" s="32"/>
       <c r="K21" s="31"/>
-      <c r="L21" s="31"/>
+      <c r="L21" s="44"/>
       <c r="M21" s="32"/>
       <c r="N21" s="32"/>
       <c r="O21" s="31"/>
@@ -1646,7 +1676,7 @@
       <c r="I22" s="31"/>
       <c r="J22" s="32"/>
       <c r="K22" s="31"/>
-      <c r="L22" s="31"/>
+      <c r="L22" s="44"/>
       <c r="M22" s="32"/>
       <c r="N22" s="32"/>
       <c r="O22" s="31"/>
@@ -1684,7 +1714,7 @@
       <c r="I23" s="31"/>
       <c r="J23" s="32"/>
       <c r="K23" s="31"/>
-      <c r="L23" s="31"/>
+      <c r="L23" s="44"/>
       <c r="M23" s="32"/>
       <c r="N23" s="32"/>
       <c r="O23" s="31"/>
@@ -1722,7 +1752,7 @@
       <c r="I24" s="31"/>
       <c r="J24" s="32"/>
       <c r="K24" s="31"/>
-      <c r="L24" s="31"/>
+      <c r="L24" s="44"/>
       <c r="M24" s="32"/>
       <c r="N24" s="32"/>
       <c r="O24" s="31"/>
@@ -1760,7 +1790,7 @@
       <c r="I25" s="31"/>
       <c r="J25" s="32"/>
       <c r="K25" s="31"/>
-      <c r="L25" s="31"/>
+      <c r="L25" s="44"/>
       <c r="M25" s="32"/>
       <c r="N25" s="32"/>
       <c r="O25" s="31"/>
@@ -1798,7 +1828,7 @@
       <c r="I26" s="31"/>
       <c r="J26" s="32"/>
       <c r="K26" s="31"/>
-      <c r="L26" s="31"/>
+      <c r="L26" s="44"/>
       <c r="M26" s="32"/>
       <c r="N26" s="32"/>
       <c r="O26" s="31"/>
@@ -1836,7 +1866,7 @@
       <c r="I27" s="31"/>
       <c r="J27" s="32"/>
       <c r="K27" s="31"/>
-      <c r="L27" s="31"/>
+      <c r="L27" s="44"/>
       <c r="M27" s="32"/>
       <c r="N27" s="32"/>
       <c r="O27" s="31"/>
@@ -1874,7 +1904,7 @@
       <c r="I28" s="31"/>
       <c r="J28" s="32"/>
       <c r="K28" s="31"/>
-      <c r="L28" s="31"/>
+      <c r="L28" s="44"/>
       <c r="M28" s="32"/>
       <c r="N28" s="32"/>
       <c r="O28" s="31"/>
@@ -1912,7 +1942,7 @@
       <c r="I29" s="31"/>
       <c r="J29" s="32"/>
       <c r="K29" s="31"/>
-      <c r="L29" s="31"/>
+      <c r="L29" s="44"/>
       <c r="M29" s="32"/>
       <c r="N29" s="32"/>
       <c r="O29" s="31"/>
@@ -1950,7 +1980,7 @@
       <c r="I30" s="31"/>
       <c r="J30" s="32"/>
       <c r="K30" s="31"/>
-      <c r="L30" s="31"/>
+      <c r="L30" s="44"/>
       <c r="M30" s="32"/>
       <c r="N30" s="32"/>
       <c r="O30" s="31"/>
@@ -1988,7 +2018,7 @@
       <c r="I31" s="17"/>
       <c r="J31" s="18"/>
       <c r="K31" s="17"/>
-      <c r="L31" s="17"/>
+      <c r="L31" s="45"/>
       <c r="M31" s="18"/>
       <c r="N31" s="18"/>
       <c r="O31" s="17"/>
@@ -2013,7 +2043,7 @@
       <c r="I32" s="17"/>
       <c r="J32" s="18"/>
       <c r="K32" s="17"/>
-      <c r="L32" s="17"/>
+      <c r="L32" s="45"/>
       <c r="M32" s="18"/>
       <c r="N32" s="18"/>
       <c r="O32" s="17"/>
@@ -2038,7 +2068,7 @@
       <c r="I33" s="17"/>
       <c r="J33" s="18"/>
       <c r="K33" s="17"/>
-      <c r="L33" s="17"/>
+      <c r="L33" s="45"/>
       <c r="M33" s="18"/>
       <c r="N33" s="18"/>
       <c r="O33" s="17"/>
@@ -2063,7 +2093,7 @@
       <c r="I34" s="17"/>
       <c r="J34" s="18"/>
       <c r="K34" s="17"/>
-      <c r="L34" s="17"/>
+      <c r="L34" s="45"/>
       <c r="M34" s="18"/>
       <c r="N34" s="18"/>
       <c r="O34" s="17"/>
@@ -2088,7 +2118,7 @@
       <c r="I35" s="17"/>
       <c r="J35" s="18"/>
       <c r="K35" s="17"/>
-      <c r="L35" s="17"/>
+      <c r="L35" s="45"/>
       <c r="M35" s="18"/>
       <c r="N35" s="18"/>
       <c r="O35" s="17"/>
@@ -2113,7 +2143,7 @@
       <c r="I36" s="17"/>
       <c r="J36" s="18"/>
       <c r="K36" s="17"/>
-      <c r="L36" s="17"/>
+      <c r="L36" s="45"/>
       <c r="M36" s="18"/>
       <c r="N36" s="18"/>
       <c r="O36" s="17"/>
@@ -2138,7 +2168,7 @@
       <c r="I37" s="17"/>
       <c r="J37" s="18"/>
       <c r="K37" s="17"/>
-      <c r="L37" s="17"/>
+      <c r="L37" s="45"/>
       <c r="M37" s="18"/>
       <c r="N37" s="18"/>
       <c r="O37" s="17"/>
@@ -2163,7 +2193,7 @@
       <c r="I38" s="17"/>
       <c r="J38" s="18"/>
       <c r="K38" s="17"/>
-      <c r="L38" s="17"/>
+      <c r="L38" s="45"/>
       <c r="M38" s="18"/>
       <c r="N38" s="18"/>
       <c r="O38" s="17"/>
@@ -2188,7 +2218,7 @@
       <c r="I39" s="17"/>
       <c r="J39" s="18"/>
       <c r="K39" s="17"/>
-      <c r="L39" s="17"/>
+      <c r="L39" s="45"/>
       <c r="M39" s="18"/>
       <c r="N39" s="18"/>
       <c r="O39" s="17"/>
@@ -2213,7 +2243,7 @@
       <c r="I40" s="17"/>
       <c r="J40" s="18"/>
       <c r="K40" s="17"/>
-      <c r="L40" s="17"/>
+      <c r="L40" s="45"/>
       <c r="M40" s="18"/>
       <c r="N40" s="18"/>
       <c r="O40" s="17"/>
@@ -2238,7 +2268,7 @@
       <c r="I41" s="17"/>
       <c r="J41" s="18"/>
       <c r="K41" s="17"/>
-      <c r="L41" s="17"/>
+      <c r="L41" s="45"/>
       <c r="M41" s="18"/>
       <c r="N41" s="18"/>
       <c r="O41" s="17"/>
@@ -2263,7 +2293,7 @@
       <c r="I42" s="17"/>
       <c r="J42" s="18"/>
       <c r="K42" s="17"/>
-      <c r="L42" s="17"/>
+      <c r="L42" s="45"/>
       <c r="M42" s="18"/>
       <c r="N42" s="18"/>
       <c r="O42" s="17"/>
@@ -2288,7 +2318,7 @@
       <c r="I43" s="17"/>
       <c r="J43" s="18"/>
       <c r="K43" s="17"/>
-      <c r="L43" s="17"/>
+      <c r="L43" s="45"/>
       <c r="M43" s="18"/>
       <c r="N43" s="18"/>
       <c r="O43" s="17"/>
@@ -2313,7 +2343,7 @@
       <c r="I44" s="17"/>
       <c r="J44" s="18"/>
       <c r="K44" s="17"/>
-      <c r="L44" s="17"/>
+      <c r="L44" s="45"/>
       <c r="M44" s="18"/>
       <c r="N44" s="18"/>
       <c r="O44" s="17"/>
@@ -2338,7 +2368,7 @@
       <c r="I45" s="17"/>
       <c r="J45" s="18"/>
       <c r="K45" s="17"/>
-      <c r="L45" s="17"/>
+      <c r="L45" s="45"/>
       <c r="M45" s="18"/>
       <c r="N45" s="18"/>
       <c r="O45" s="17"/>
@@ -2363,7 +2393,7 @@
       <c r="I46" s="17"/>
       <c r="J46" s="18"/>
       <c r="K46" s="17"/>
-      <c r="L46" s="17"/>
+      <c r="L46" s="45"/>
       <c r="M46" s="18"/>
       <c r="N46" s="18"/>
       <c r="O46" s="17"/>
@@ -2388,7 +2418,7 @@
       <c r="I47" s="17"/>
       <c r="J47" s="18"/>
       <c r="K47" s="17"/>
-      <c r="L47" s="17"/>
+      <c r="L47" s="45"/>
       <c r="M47" s="18"/>
       <c r="N47" s="18"/>
       <c r="O47" s="17"/>
@@ -2413,7 +2443,7 @@
       <c r="I48" s="17"/>
       <c r="J48" s="18"/>
       <c r="K48" s="17"/>
-      <c r="L48" s="17"/>
+      <c r="L48" s="45"/>
       <c r="M48" s="18"/>
       <c r="N48" s="18"/>
       <c r="O48" s="17"/>
@@ -2438,7 +2468,7 @@
       <c r="I49" s="17"/>
       <c r="J49" s="18"/>
       <c r="K49" s="17"/>
-      <c r="L49" s="17"/>
+      <c r="L49" s="45"/>
       <c r="M49" s="18"/>
       <c r="N49" s="18"/>
       <c r="O49" s="17"/>
@@ -2463,7 +2493,7 @@
       <c r="I50" s="17"/>
       <c r="J50" s="18"/>
       <c r="K50" s="17"/>
-      <c r="L50" s="17"/>
+      <c r="L50" s="45"/>
       <c r="M50" s="18"/>
       <c r="N50" s="18"/>
       <c r="O50" s="17"/>
@@ -2488,7 +2518,7 @@
       <c r="I51" s="17"/>
       <c r="J51" s="18"/>
       <c r="K51" s="17"/>
-      <c r="L51" s="17"/>
+      <c r="L51" s="45"/>
       <c r="M51" s="18"/>
       <c r="N51" s="18"/>
       <c r="O51" s="17"/>
@@ -2513,7 +2543,7 @@
       <c r="I52" s="17"/>
       <c r="J52" s="18"/>
       <c r="K52" s="17"/>
-      <c r="L52" s="17"/>
+      <c r="L52" s="45"/>
       <c r="M52" s="18"/>
       <c r="N52" s="18"/>
       <c r="O52" s="17"/>
@@ -2538,7 +2568,7 @@
       <c r="I53" s="17"/>
       <c r="J53" s="18"/>
       <c r="K53" s="17"/>
-      <c r="L53" s="17"/>
+      <c r="L53" s="45"/>
       <c r="M53" s="18"/>
       <c r="N53" s="18"/>
       <c r="O53" s="17"/>
@@ -2563,7 +2593,7 @@
       <c r="I54" s="17"/>
       <c r="J54" s="18"/>
       <c r="K54" s="17"/>
-      <c r="L54" s="17"/>
+      <c r="L54" s="45"/>
       <c r="M54" s="18"/>
       <c r="N54" s="18"/>
       <c r="O54" s="17"/>
@@ -2588,7 +2618,7 @@
       <c r="I55" s="17"/>
       <c r="J55" s="18"/>
       <c r="K55" s="17"/>
-      <c r="L55" s="17"/>
+      <c r="L55" s="45"/>
       <c r="M55" s="18"/>
       <c r="N55" s="18"/>
       <c r="O55" s="17"/>
@@ -2613,7 +2643,7 @@
       <c r="I56" s="17"/>
       <c r="J56" s="18"/>
       <c r="K56" s="17"/>
-      <c r="L56" s="17"/>
+      <c r="L56" s="45"/>
       <c r="M56" s="18"/>
       <c r="N56" s="18"/>
       <c r="O56" s="17"/>
@@ -2638,7 +2668,7 @@
       <c r="I57" s="17"/>
       <c r="J57" s="18"/>
       <c r="K57" s="17"/>
-      <c r="L57" s="17"/>
+      <c r="L57" s="45"/>
       <c r="M57" s="18"/>
       <c r="N57" s="18"/>
       <c r="O57" s="17"/>
@@ -2663,7 +2693,7 @@
       <c r="I58" s="17"/>
       <c r="J58" s="18"/>
       <c r="K58" s="17"/>
-      <c r="L58" s="17"/>
+      <c r="L58" s="45"/>
       <c r="M58" s="18"/>
       <c r="N58" s="18"/>
       <c r="O58" s="17"/>
@@ -2688,7 +2718,7 @@
       <c r="I59" s="17"/>
       <c r="J59" s="18"/>
       <c r="K59" s="17"/>
-      <c r="L59" s="17"/>
+      <c r="L59" s="45"/>
       <c r="M59" s="18"/>
       <c r="N59" s="18"/>
       <c r="O59" s="17"/>
@@ -2713,7 +2743,7 @@
       <c r="I60" s="17"/>
       <c r="J60" s="18"/>
       <c r="K60" s="17"/>
-      <c r="L60" s="17"/>
+      <c r="L60" s="45"/>
       <c r="M60" s="18"/>
       <c r="N60" s="18"/>
       <c r="O60" s="17"/>
@@ -2738,7 +2768,7 @@
       <c r="I61" s="17"/>
       <c r="J61" s="18"/>
       <c r="K61" s="17"/>
-      <c r="L61" s="17"/>
+      <c r="L61" s="45"/>
       <c r="M61" s="18"/>
       <c r="N61" s="18"/>
       <c r="O61" s="17"/>
@@ -2763,7 +2793,7 @@
       <c r="I62" s="17"/>
       <c r="J62" s="18"/>
       <c r="K62" s="17"/>
-      <c r="L62" s="17"/>
+      <c r="L62" s="45"/>
       <c r="M62" s="18"/>
       <c r="N62" s="18"/>
       <c r="O62" s="17"/>
@@ -2788,7 +2818,7 @@
       <c r="I63" s="17"/>
       <c r="J63" s="18"/>
       <c r="K63" s="17"/>
-      <c r="L63" s="17"/>
+      <c r="L63" s="45"/>
       <c r="M63" s="18"/>
       <c r="N63" s="18"/>
       <c r="O63" s="17"/>
@@ -2813,7 +2843,7 @@
       <c r="I64" s="17"/>
       <c r="J64" s="18"/>
       <c r="K64" s="17"/>
-      <c r="L64" s="17"/>
+      <c r="L64" s="45"/>
       <c r="M64" s="18"/>
       <c r="N64" s="18"/>
       <c r="O64" s="17"/>
@@ -2838,7 +2868,7 @@
       <c r="I65" s="17"/>
       <c r="J65" s="18"/>
       <c r="K65" s="17"/>
-      <c r="L65" s="17"/>
+      <c r="L65" s="45"/>
       <c r="M65" s="18"/>
       <c r="N65" s="18"/>
       <c r="O65" s="17"/>
@@ -2863,7 +2893,7 @@
       <c r="I66" s="17"/>
       <c r="J66" s="18"/>
       <c r="K66" s="17"/>
-      <c r="L66" s="17"/>
+      <c r="L66" s="45"/>
       <c r="M66" s="18"/>
       <c r="N66" s="18"/>
       <c r="O66" s="17"/>
@@ -2888,7 +2918,7 @@
       <c r="I67" s="17"/>
       <c r="J67" s="18"/>
       <c r="K67" s="17"/>
-      <c r="L67" s="17"/>
+      <c r="L67" s="45"/>
       <c r="M67" s="18"/>
       <c r="N67" s="18"/>
       <c r="O67" s="17"/>
@@ -2913,7 +2943,7 @@
       <c r="I68" s="17"/>
       <c r="J68" s="18"/>
       <c r="K68" s="17"/>
-      <c r="L68" s="17"/>
+      <c r="L68" s="45"/>
       <c r="M68" s="18"/>
       <c r="N68" s="18"/>
       <c r="O68" s="17"/>
@@ -2938,7 +2968,7 @@
       <c r="I69" s="17"/>
       <c r="J69" s="18"/>
       <c r="K69" s="17"/>
-      <c r="L69" s="17"/>
+      <c r="L69" s="45"/>
       <c r="M69" s="18"/>
       <c r="N69" s="18"/>
       <c r="O69" s="17"/>
@@ -2963,7 +2993,7 @@
       <c r="I70" s="17"/>
       <c r="J70" s="18"/>
       <c r="K70" s="17"/>
-      <c r="L70" s="17"/>
+      <c r="L70" s="45"/>
       <c r="M70" s="18"/>
       <c r="N70" s="18"/>
       <c r="O70" s="17"/>
@@ -2988,7 +3018,7 @@
       <c r="I71" s="17"/>
       <c r="J71" s="18"/>
       <c r="K71" s="17"/>
-      <c r="L71" s="17"/>
+      <c r="L71" s="45"/>
       <c r="M71" s="18"/>
       <c r="N71" s="18"/>
       <c r="O71" s="17"/>
@@ -3013,7 +3043,7 @@
       <c r="I72" s="17"/>
       <c r="J72" s="18"/>
       <c r="K72" s="17"/>
-      <c r="L72" s="17"/>
+      <c r="L72" s="45"/>
       <c r="M72" s="18"/>
       <c r="N72" s="18"/>
       <c r="O72" s="17"/>
@@ -3038,7 +3068,7 @@
       <c r="I73" s="17"/>
       <c r="J73" s="18"/>
       <c r="K73" s="17"/>
-      <c r="L73" s="17"/>
+      <c r="L73" s="45"/>
       <c r="M73" s="18"/>
       <c r="N73" s="18"/>
       <c r="O73" s="17"/>
@@ -3063,7 +3093,7 @@
       <c r="I74" s="17"/>
       <c r="J74" s="18"/>
       <c r="K74" s="17"/>
-      <c r="L74" s="17"/>
+      <c r="L74" s="45"/>
       <c r="M74" s="18"/>
       <c r="N74" s="18"/>
       <c r="O74" s="17"/>
@@ -3088,7 +3118,7 @@
       <c r="I75" s="17"/>
       <c r="J75" s="18"/>
       <c r="K75" s="17"/>
-      <c r="L75" s="17"/>
+      <c r="L75" s="45"/>
       <c r="M75" s="18"/>
       <c r="N75" s="18"/>
       <c r="O75" s="17"/>
@@ -3113,7 +3143,7 @@
       <c r="I76" s="17"/>
       <c r="J76" s="18"/>
       <c r="K76" s="17"/>
-      <c r="L76" s="17"/>
+      <c r="L76" s="45"/>
       <c r="M76" s="18"/>
       <c r="N76" s="18"/>
       <c r="O76" s="17"/>
@@ -3138,7 +3168,7 @@
       <c r="I77" s="17"/>
       <c r="J77" s="18"/>
       <c r="K77" s="17"/>
-      <c r="L77" s="17"/>
+      <c r="L77" s="45"/>
       <c r="M77" s="18"/>
       <c r="N77" s="18"/>
       <c r="O77" s="17"/>
@@ -3163,7 +3193,7 @@
       <c r="I78" s="17"/>
       <c r="J78" s="18"/>
       <c r="K78" s="17"/>
-      <c r="L78" s="17"/>
+      <c r="L78" s="45"/>
       <c r="M78" s="18"/>
       <c r="N78" s="18"/>
       <c r="O78" s="17"/>
@@ -3188,7 +3218,7 @@
       <c r="I79" s="17"/>
       <c r="J79" s="18"/>
       <c r="K79" s="17"/>
-      <c r="L79" s="17"/>
+      <c r="L79" s="45"/>
       <c r="M79" s="18"/>
       <c r="N79" s="18"/>
       <c r="O79" s="17"/>
@@ -3213,7 +3243,7 @@
       <c r="I80" s="17"/>
       <c r="J80" s="18"/>
       <c r="K80" s="17"/>
-      <c r="L80" s="17"/>
+      <c r="L80" s="45"/>
       <c r="M80" s="18"/>
       <c r="N80" s="18"/>
       <c r="O80" s="17"/>
@@ -3238,7 +3268,7 @@
       <c r="I81" s="17"/>
       <c r="J81" s="18"/>
       <c r="K81" s="17"/>
-      <c r="L81" s="17"/>
+      <c r="L81" s="45"/>
       <c r="M81" s="18"/>
       <c r="N81" s="18"/>
       <c r="O81" s="17"/>
@@ -3263,7 +3293,7 @@
       <c r="I82" s="17"/>
       <c r="J82" s="18"/>
       <c r="K82" s="17"/>
-      <c r="L82" s="17"/>
+      <c r="L82" s="45"/>
       <c r="M82" s="18"/>
       <c r="N82" s="18"/>
       <c r="O82" s="17"/>
@@ -3288,7 +3318,7 @@
       <c r="I83" s="17"/>
       <c r="J83" s="18"/>
       <c r="K83" s="17"/>
-      <c r="L83" s="17"/>
+      <c r="L83" s="45"/>
       <c r="M83" s="18"/>
       <c r="N83" s="18"/>
       <c r="O83" s="17"/>
@@ -3313,7 +3343,7 @@
       <c r="I84" s="17"/>
       <c r="J84" s="18"/>
       <c r="K84" s="17"/>
-      <c r="L84" s="17"/>
+      <c r="L84" s="45"/>
       <c r="M84" s="18"/>
       <c r="N84" s="18"/>
       <c r="O84" s="17"/>
@@ -3338,7 +3368,7 @@
       <c r="I85" s="17"/>
       <c r="J85" s="18"/>
       <c r="K85" s="17"/>
-      <c r="L85" s="17"/>
+      <c r="L85" s="45"/>
       <c r="M85" s="18"/>
       <c r="N85" s="18"/>
       <c r="O85" s="17"/>
@@ -3363,7 +3393,7 @@
       <c r="I86" s="17"/>
       <c r="J86" s="18"/>
       <c r="K86" s="17"/>
-      <c r="L86" s="17"/>
+      <c r="L86" s="45"/>
       <c r="M86" s="18"/>
       <c r="N86" s="18"/>
       <c r="O86" s="17"/>
@@ -3388,7 +3418,7 @@
       <c r="I87" s="17"/>
       <c r="J87" s="18"/>
       <c r="K87" s="17"/>
-      <c r="L87" s="17"/>
+      <c r="L87" s="45"/>
       <c r="M87" s="18"/>
       <c r="N87" s="18"/>
       <c r="O87" s="17"/>
@@ -3413,7 +3443,7 @@
       <c r="I88" s="17"/>
       <c r="J88" s="18"/>
       <c r="K88" s="17"/>
-      <c r="L88" s="17"/>
+      <c r="L88" s="45"/>
       <c r="M88" s="18"/>
       <c r="N88" s="18"/>
       <c r="O88" s="17"/>
@@ -3438,7 +3468,7 @@
       <c r="I89" s="17"/>
       <c r="J89" s="18"/>
       <c r="K89" s="17"/>
-      <c r="L89" s="17"/>
+      <c r="L89" s="45"/>
       <c r="M89" s="18"/>
       <c r="N89" s="18"/>
       <c r="O89" s="17"/>
@@ -3463,7 +3493,7 @@
       <c r="I90" s="17"/>
       <c r="J90" s="18"/>
       <c r="K90" s="17"/>
-      <c r="L90" s="17"/>
+      <c r="L90" s="45"/>
       <c r="M90" s="18"/>
       <c r="N90" s="18"/>
       <c r="O90" s="17"/>
@@ -3488,7 +3518,7 @@
       <c r="I91" s="17"/>
       <c r="J91" s="18"/>
       <c r="K91" s="17"/>
-      <c r="L91" s="17"/>
+      <c r="L91" s="45"/>
       <c r="M91" s="18"/>
       <c r="N91" s="18"/>
       <c r="O91" s="17"/>
@@ -3513,7 +3543,7 @@
       <c r="I92" s="17"/>
       <c r="J92" s="18"/>
       <c r="K92" s="17"/>
-      <c r="L92" s="17"/>
+      <c r="L92" s="45"/>
       <c r="M92" s="18"/>
       <c r="N92" s="18"/>
       <c r="O92" s="17"/>
@@ -3538,7 +3568,7 @@
       <c r="I93" s="17"/>
       <c r="J93" s="18"/>
       <c r="K93" s="17"/>
-      <c r="L93" s="17"/>
+      <c r="L93" s="45"/>
       <c r="M93" s="18"/>
       <c r="N93" s="18"/>
       <c r="O93" s="17"/>
@@ -3563,7 +3593,7 @@
       <c r="I94" s="17"/>
       <c r="J94" s="18"/>
       <c r="K94" s="17"/>
-      <c r="L94" s="17"/>
+      <c r="L94" s="45"/>
       <c r="M94" s="18"/>
       <c r="N94" s="18"/>
       <c r="O94" s="17"/>
@@ -3588,7 +3618,7 @@
       <c r="I95" s="17"/>
       <c r="J95" s="18"/>
       <c r="K95" s="17"/>
-      <c r="L95" s="17"/>
+      <c r="L95" s="45"/>
       <c r="M95" s="18"/>
       <c r="N95" s="18"/>
       <c r="O95" s="17"/>
@@ -3613,7 +3643,7 @@
       <c r="I96" s="17"/>
       <c r="J96" s="18"/>
       <c r="K96" s="17"/>
-      <c r="L96" s="17"/>
+      <c r="L96" s="45"/>
       <c r="M96" s="18"/>
       <c r="N96" s="18"/>
       <c r="O96" s="17"/>
@@ -3638,7 +3668,7 @@
       <c r="I97" s="17"/>
       <c r="J97" s="18"/>
       <c r="K97" s="17"/>
-      <c r="L97" s="17"/>
+      <c r="L97" s="45"/>
       <c r="M97" s="18"/>
       <c r="N97" s="18"/>
       <c r="O97" s="17"/>
@@ -3663,7 +3693,7 @@
       <c r="I98" s="17"/>
       <c r="J98" s="18"/>
       <c r="K98" s="17"/>
-      <c r="L98" s="17"/>
+      <c r="L98" s="45"/>
       <c r="M98" s="18"/>
       <c r="N98" s="18"/>
       <c r="O98" s="17"/>
@@ -3688,7 +3718,7 @@
       <c r="I99" s="17"/>
       <c r="J99" s="18"/>
       <c r="K99" s="17"/>
-      <c r="L99" s="17"/>
+      <c r="L99" s="45"/>
       <c r="M99" s="18"/>
       <c r="N99" s="18"/>
       <c r="O99" s="17"/>
@@ -3713,7 +3743,7 @@
       <c r="I100" s="17"/>
       <c r="J100" s="18"/>
       <c r="K100" s="17"/>
-      <c r="L100" s="17"/>
+      <c r="L100" s="45"/>
       <c r="M100" s="18"/>
       <c r="N100" s="18"/>
       <c r="O100" s="17"/>
@@ -3738,7 +3768,7 @@
       <c r="I101" s="17"/>
       <c r="J101" s="18"/>
       <c r="K101" s="17"/>
-      <c r="L101" s="17"/>
+      <c r="L101" s="45"/>
       <c r="M101" s="18"/>
       <c r="N101" s="18"/>
       <c r="O101" s="17"/>
@@ -3763,7 +3793,7 @@
       <c r="I102" s="17"/>
       <c r="J102" s="18"/>
       <c r="K102" s="17"/>
-      <c r="L102" s="17"/>
+      <c r="L102" s="45"/>
       <c r="M102" s="18"/>
       <c r="N102" s="18"/>
       <c r="O102" s="17"/>
@@ -3788,7 +3818,7 @@
       <c r="I103" s="17"/>
       <c r="J103" s="18"/>
       <c r="K103" s="17"/>
-      <c r="L103" s="17"/>
+      <c r="L103" s="45"/>
       <c r="M103" s="18"/>
       <c r="N103" s="18"/>
       <c r="O103" s="17"/>
@@ -3813,7 +3843,7 @@
       <c r="I104" s="17"/>
       <c r="J104" s="18"/>
       <c r="K104" s="17"/>
-      <c r="L104" s="17"/>
+      <c r="L104" s="45"/>
       <c r="M104" s="18"/>
       <c r="N104" s="18"/>
       <c r="O104" s="17"/>
@@ -3838,7 +3868,7 @@
       <c r="I105" s="17"/>
       <c r="J105" s="18"/>
       <c r="K105" s="17"/>
-      <c r="L105" s="17"/>
+      <c r="L105" s="45"/>
       <c r="M105" s="18"/>
       <c r="N105" s="18"/>
       <c r="O105" s="17"/>
@@ -3863,7 +3893,7 @@
       <c r="I106" s="17"/>
       <c r="J106" s="18"/>
       <c r="K106" s="17"/>
-      <c r="L106" s="17"/>
+      <c r="L106" s="45"/>
       <c r="M106" s="18"/>
       <c r="N106" s="18"/>
       <c r="O106" s="17"/>
@@ -3888,7 +3918,7 @@
       <c r="I107" s="17"/>
       <c r="J107" s="18"/>
       <c r="K107" s="17"/>
-      <c r="L107" s="17"/>
+      <c r="L107" s="45"/>
       <c r="M107" s="18"/>
       <c r="N107" s="18"/>
       <c r="O107" s="17"/>
@@ -3913,7 +3943,7 @@
       <c r="I108" s="17"/>
       <c r="J108" s="18"/>
       <c r="K108" s="17"/>
-      <c r="L108" s="17"/>
+      <c r="L108" s="45"/>
       <c r="M108" s="18"/>
       <c r="N108" s="18"/>
       <c r="O108" s="17"/>
@@ -3938,7 +3968,7 @@
       <c r="I109" s="17"/>
       <c r="J109" s="18"/>
       <c r="K109" s="17"/>
-      <c r="L109" s="17"/>
+      <c r="L109" s="45"/>
       <c r="M109" s="18"/>
       <c r="N109" s="18"/>
       <c r="O109" s="17"/>
@@ -3963,7 +3993,7 @@
       <c r="I110" s="17"/>
       <c r="J110" s="18"/>
       <c r="K110" s="17"/>
-      <c r="L110" s="17"/>
+      <c r="L110" s="45"/>
       <c r="M110" s="18"/>
       <c r="N110" s="18"/>
       <c r="O110" s="17"/>
@@ -3988,7 +4018,7 @@
       <c r="I111" s="17"/>
       <c r="J111" s="18"/>
       <c r="K111" s="17"/>
-      <c r="L111" s="17"/>
+      <c r="L111" s="45"/>
       <c r="M111" s="18"/>
       <c r="N111" s="18"/>
       <c r="O111" s="17"/>
@@ -4013,7 +4043,7 @@
       <c r="I112" s="17"/>
       <c r="J112" s="18"/>
       <c r="K112" s="17"/>
-      <c r="L112" s="17"/>
+      <c r="L112" s="45"/>
       <c r="M112" s="18"/>
       <c r="N112" s="18"/>
       <c r="O112" s="17"/>
@@ -4038,7 +4068,7 @@
       <c r="I113" s="17"/>
       <c r="J113" s="18"/>
       <c r="K113" s="17"/>
-      <c r="L113" s="17"/>
+      <c r="L113" s="45"/>
       <c r="M113" s="18"/>
       <c r="N113" s="18"/>
       <c r="O113" s="17"/>
@@ -4063,7 +4093,7 @@
       <c r="I114" s="17"/>
       <c r="J114" s="18"/>
       <c r="K114" s="17"/>
-      <c r="L114" s="17"/>
+      <c r="L114" s="45"/>
       <c r="M114" s="18"/>
       <c r="N114" s="18"/>
       <c r="O114" s="17"/>
@@ -4088,7 +4118,7 @@
       <c r="I115" s="17"/>
       <c r="J115" s="18"/>
       <c r="K115" s="17"/>
-      <c r="L115" s="17"/>
+      <c r="L115" s="45"/>
       <c r="M115" s="18"/>
       <c r="N115" s="18"/>
       <c r="O115" s="17"/>
@@ -4113,7 +4143,7 @@
       <c r="I116" s="17"/>
       <c r="J116" s="18"/>
       <c r="K116" s="17"/>
-      <c r="L116" s="17"/>
+      <c r="L116" s="45"/>
       <c r="M116" s="18"/>
       <c r="N116" s="18"/>
       <c r="O116" s="17"/>
@@ -4138,7 +4168,7 @@
       <c r="I117" s="17"/>
       <c r="J117" s="18"/>
       <c r="K117" s="17"/>
-      <c r="L117" s="17"/>
+      <c r="L117" s="45"/>
       <c r="M117" s="18"/>
       <c r="N117" s="18"/>
       <c r="O117" s="17"/>
@@ -4163,7 +4193,7 @@
       <c r="I118" s="17"/>
       <c r="J118" s="18"/>
       <c r="K118" s="17"/>
-      <c r="L118" s="17"/>
+      <c r="L118" s="45"/>
       <c r="M118" s="18"/>
       <c r="N118" s="18"/>
       <c r="O118" s="17"/>
@@ -4188,7 +4218,7 @@
       <c r="I119" s="17"/>
       <c r="J119" s="18"/>
       <c r="K119" s="17"/>
-      <c r="L119" s="17"/>
+      <c r="L119" s="45"/>
       <c r="M119" s="18"/>
       <c r="N119" s="18"/>
       <c r="O119" s="17"/>
@@ -4213,7 +4243,7 @@
       <c r="I120" s="17"/>
       <c r="J120" s="18"/>
       <c r="K120" s="17"/>
-      <c r="L120" s="17"/>
+      <c r="L120" s="45"/>
       <c r="M120" s="18"/>
       <c r="N120" s="18"/>
       <c r="O120" s="17"/>
@@ -4238,7 +4268,7 @@
       <c r="I121" s="17"/>
       <c r="J121" s="18"/>
       <c r="K121" s="17"/>
-      <c r="L121" s="17"/>
+      <c r="L121" s="45"/>
       <c r="M121" s="18"/>
       <c r="N121" s="18"/>
       <c r="O121" s="17"/>
@@ -4263,7 +4293,7 @@
       <c r="I122" s="17"/>
       <c r="J122" s="18"/>
       <c r="K122" s="17"/>
-      <c r="L122" s="17"/>
+      <c r="L122" s="45"/>
       <c r="M122" s="18"/>
       <c r="N122" s="18"/>
       <c r="O122" s="17"/>
@@ -4288,7 +4318,7 @@
       <c r="I123" s="17"/>
       <c r="J123" s="18"/>
       <c r="K123" s="17"/>
-      <c r="L123" s="17"/>
+      <c r="L123" s="45"/>
       <c r="M123" s="18"/>
       <c r="N123" s="18"/>
       <c r="O123" s="17"/>
@@ -4313,7 +4343,7 @@
       <c r="I124" s="17"/>
       <c r="J124" s="18"/>
       <c r="K124" s="17"/>
-      <c r="L124" s="17"/>
+      <c r="L124" s="45"/>
       <c r="M124" s="18"/>
       <c r="N124" s="18"/>
       <c r="O124" s="17"/>
@@ -4338,7 +4368,7 @@
       <c r="I125" s="17"/>
       <c r="J125" s="18"/>
       <c r="K125" s="17"/>
-      <c r="L125" s="17"/>
+      <c r="L125" s="45"/>
       <c r="M125" s="18"/>
       <c r="N125" s="18"/>
       <c r="O125" s="17"/>
@@ -4363,7 +4393,7 @@
       <c r="I126" s="17"/>
       <c r="J126" s="18"/>
       <c r="K126" s="17"/>
-      <c r="L126" s="17"/>
+      <c r="L126" s="45"/>
       <c r="M126" s="18"/>
       <c r="N126" s="18"/>
       <c r="O126" s="17"/>
@@ -4388,7 +4418,7 @@
       <c r="I127" s="17"/>
       <c r="J127" s="18"/>
       <c r="K127" s="17"/>
-      <c r="L127" s="17"/>
+      <c r="L127" s="45"/>
       <c r="M127" s="18"/>
       <c r="N127" s="18"/>
       <c r="O127" s="17"/>
@@ -4413,7 +4443,7 @@
       <c r="I128" s="17"/>
       <c r="J128" s="18"/>
       <c r="K128" s="17"/>
-      <c r="L128" s="17"/>
+      <c r="L128" s="45"/>
       <c r="M128" s="18"/>
       <c r="N128" s="18"/>
       <c r="O128" s="17"/>
@@ -4438,7 +4468,7 @@
       <c r="I129" s="17"/>
       <c r="J129" s="18"/>
       <c r="K129" s="17"/>
-      <c r="L129" s="17"/>
+      <c r="L129" s="45"/>
       <c r="M129" s="18"/>
       <c r="N129" s="18"/>
       <c r="O129" s="17"/>
@@ -4463,7 +4493,7 @@
       <c r="I130" s="17"/>
       <c r="J130" s="18"/>
       <c r="K130" s="17"/>
-      <c r="L130" s="17"/>
+      <c r="L130" s="45"/>
       <c r="M130" s="18"/>
       <c r="N130" s="18"/>
       <c r="O130" s="17"/>
@@ -4488,7 +4518,7 @@
       <c r="I131" s="17"/>
       <c r="J131" s="18"/>
       <c r="K131" s="17"/>
-      <c r="L131" s="17"/>
+      <c r="L131" s="45"/>
       <c r="M131" s="18"/>
       <c r="N131" s="18"/>
       <c r="O131" s="17"/>
@@ -4513,7 +4543,7 @@
       <c r="I132" s="17"/>
       <c r="J132" s="18"/>
       <c r="K132" s="17"/>
-      <c r="L132" s="17"/>
+      <c r="L132" s="45"/>
       <c r="M132" s="18"/>
       <c r="N132" s="18"/>
       <c r="O132" s="17"/>
@@ -4538,7 +4568,7 @@
       <c r="I133" s="17"/>
       <c r="J133" s="18"/>
       <c r="K133" s="17"/>
-      <c r="L133" s="17"/>
+      <c r="L133" s="45"/>
       <c r="M133" s="18"/>
       <c r="N133" s="18"/>
       <c r="O133" s="17"/>
@@ -4563,7 +4593,7 @@
       <c r="I134" s="17"/>
       <c r="J134" s="18"/>
       <c r="K134" s="17"/>
-      <c r="L134" s="17"/>
+      <c r="L134" s="45"/>
       <c r="M134" s="18"/>
       <c r="N134" s="18"/>
       <c r="O134" s="17"/>
@@ -4588,7 +4618,7 @@
       <c r="I135" s="17"/>
       <c r="J135" s="18"/>
       <c r="K135" s="17"/>
-      <c r="L135" s="17"/>
+      <c r="L135" s="45"/>
       <c r="M135" s="18"/>
       <c r="N135" s="18"/>
       <c r="O135" s="17"/>
@@ -4613,7 +4643,7 @@
       <c r="I136" s="17"/>
       <c r="J136" s="18"/>
       <c r="K136" s="17"/>
-      <c r="L136" s="17"/>
+      <c r="L136" s="45"/>
       <c r="M136" s="18"/>
       <c r="N136" s="18"/>
       <c r="O136" s="17"/>
@@ -4638,7 +4668,7 @@
       <c r="I137" s="17"/>
       <c r="J137" s="18"/>
       <c r="K137" s="17"/>
-      <c r="L137" s="17"/>
+      <c r="L137" s="45"/>
       <c r="M137" s="18"/>
       <c r="N137" s="18"/>
       <c r="O137" s="17"/>
@@ -4663,7 +4693,7 @@
       <c r="I138" s="17"/>
       <c r="J138" s="18"/>
       <c r="K138" s="17"/>
-      <c r="L138" s="17"/>
+      <c r="L138" s="45"/>
       <c r="M138" s="18"/>
       <c r="N138" s="18"/>
       <c r="O138" s="17"/>
@@ -4688,7 +4718,7 @@
       <c r="I139" s="17"/>
       <c r="J139" s="18"/>
       <c r="K139" s="17"/>
-      <c r="L139" s="17"/>
+      <c r="L139" s="45"/>
       <c r="M139" s="18"/>
       <c r="N139" s="18"/>
       <c r="O139" s="17"/>
@@ -4713,7 +4743,7 @@
       <c r="I140" s="17"/>
       <c r="J140" s="18"/>
       <c r="K140" s="17"/>
-      <c r="L140" s="17"/>
+      <c r="L140" s="45"/>
       <c r="M140" s="18"/>
       <c r="N140" s="18"/>
       <c r="O140" s="17"/>
@@ -4738,7 +4768,7 @@
       <c r="I141" s="17"/>
       <c r="J141" s="18"/>
       <c r="K141" s="17"/>
-      <c r="L141" s="17"/>
+      <c r="L141" s="45"/>
       <c r="M141" s="18"/>
       <c r="N141" s="18"/>
       <c r="O141" s="17"/>
@@ -4763,7 +4793,7 @@
       <c r="I142" s="17"/>
       <c r="J142" s="18"/>
       <c r="K142" s="17"/>
-      <c r="L142" s="17"/>
+      <c r="L142" s="45"/>
       <c r="M142" s="18"/>
       <c r="N142" s="18"/>
       <c r="O142" s="17"/>
@@ -4788,7 +4818,7 @@
       <c r="I143" s="17"/>
       <c r="J143" s="18"/>
       <c r="K143" s="17"/>
-      <c r="L143" s="17"/>
+      <c r="L143" s="45"/>
       <c r="M143" s="18"/>
       <c r="N143" s="18"/>
       <c r="O143" s="17"/>
@@ -4813,7 +4843,7 @@
       <c r="I144" s="17"/>
       <c r="J144" s="18"/>
       <c r="K144" s="17"/>
-      <c r="L144" s="17"/>
+      <c r="L144" s="45"/>
       <c r="M144" s="18"/>
       <c r="N144" s="18"/>
       <c r="O144" s="17"/>
@@ -4838,7 +4868,7 @@
       <c r="I145" s="17"/>
       <c r="J145" s="18"/>
       <c r="K145" s="17"/>
-      <c r="L145" s="17"/>
+      <c r="L145" s="45"/>
       <c r="M145" s="18"/>
       <c r="N145" s="18"/>
       <c r="O145" s="17"/>
@@ -4863,7 +4893,7 @@
       <c r="I146" s="17"/>
       <c r="J146" s="18"/>
       <c r="K146" s="17"/>
-      <c r="L146" s="17"/>
+      <c r="L146" s="45"/>
       <c r="M146" s="18"/>
       <c r="N146" s="18"/>
       <c r="O146" s="17"/>
@@ -4888,7 +4918,7 @@
       <c r="I147" s="17"/>
       <c r="J147" s="18"/>
       <c r="K147" s="17"/>
-      <c r="L147" s="17"/>
+      <c r="L147" s="45"/>
       <c r="M147" s="18"/>
       <c r="N147" s="18"/>
       <c r="O147" s="17"/>
@@ -4913,7 +4943,7 @@
       <c r="I148" s="17"/>
       <c r="J148" s="18"/>
       <c r="K148" s="17"/>
-      <c r="L148" s="17"/>
+      <c r="L148" s="45"/>
       <c r="M148" s="18"/>
       <c r="N148" s="18"/>
       <c r="O148" s="17"/>
@@ -4938,7 +4968,7 @@
       <c r="I149" s="17"/>
       <c r="J149" s="18"/>
       <c r="K149" s="17"/>
-      <c r="L149" s="17"/>
+      <c r="L149" s="45"/>
       <c r="M149" s="18"/>
       <c r="N149" s="18"/>
       <c r="O149" s="17"/>
@@ -4963,7 +4993,7 @@
       <c r="I150" s="17"/>
       <c r="J150" s="18"/>
       <c r="K150" s="17"/>
-      <c r="L150" s="17"/>
+      <c r="L150" s="45"/>
       <c r="M150" s="18"/>
       <c r="N150" s="18"/>
       <c r="O150" s="17"/>
@@ -4988,7 +5018,7 @@
       <c r="I151" s="17"/>
       <c r="J151" s="18"/>
       <c r="K151" s="17"/>
-      <c r="L151" s="17"/>
+      <c r="L151" s="45"/>
       <c r="M151" s="18"/>
       <c r="N151" s="18"/>
       <c r="O151" s="17"/>
@@ -5013,7 +5043,7 @@
       <c r="I152" s="17"/>
       <c r="J152" s="18"/>
       <c r="K152" s="17"/>
-      <c r="L152" s="17"/>
+      <c r="L152" s="45"/>
       <c r="M152" s="18"/>
       <c r="N152" s="18"/>
       <c r="O152" s="17"/>
@@ -5038,7 +5068,7 @@
       <c r="I153" s="17"/>
       <c r="J153" s="18"/>
       <c r="K153" s="17"/>
-      <c r="L153" s="17"/>
+      <c r="L153" s="45"/>
       <c r="M153" s="18"/>
       <c r="N153" s="18"/>
       <c r="O153" s="17"/>
@@ -5063,7 +5093,7 @@
       <c r="I154" s="17"/>
       <c r="J154" s="18"/>
       <c r="K154" s="17"/>
-      <c r="L154" s="17"/>
+      <c r="L154" s="45"/>
       <c r="M154" s="18"/>
       <c r="N154" s="18"/>
       <c r="O154" s="17"/>
@@ -5088,7 +5118,7 @@
       <c r="I155" s="17"/>
       <c r="J155" s="18"/>
       <c r="K155" s="17"/>
-      <c r="L155" s="17"/>
+      <c r="L155" s="45"/>
       <c r="M155" s="18"/>
       <c r="N155" s="18"/>
       <c r="O155" s="17"/>
@@ -5113,7 +5143,7 @@
       <c r="I156" s="17"/>
       <c r="J156" s="18"/>
       <c r="K156" s="17"/>
-      <c r="L156" s="17"/>
+      <c r="L156" s="45"/>
       <c r="M156" s="18"/>
       <c r="N156" s="18"/>
       <c r="O156" s="17"/>
@@ -5138,7 +5168,7 @@
       <c r="I157" s="17"/>
       <c r="J157" s="18"/>
       <c r="K157" s="17"/>
-      <c r="L157" s="17"/>
+      <c r="L157" s="45"/>
       <c r="M157" s="18"/>
       <c r="N157" s="18"/>
       <c r="O157" s="17"/>
@@ -5163,7 +5193,7 @@
       <c r="I158" s="17"/>
       <c r="J158" s="18"/>
       <c r="K158" s="17"/>
-      <c r="L158" s="17"/>
+      <c r="L158" s="45"/>
       <c r="M158" s="18"/>
       <c r="N158" s="18"/>
       <c r="O158" s="17"/>
@@ -5188,7 +5218,7 @@
       <c r="I159" s="17"/>
       <c r="J159" s="18"/>
       <c r="K159" s="17"/>
-      <c r="L159" s="17"/>
+      <c r="L159" s="45"/>
       <c r="M159" s="18"/>
       <c r="N159" s="18"/>
       <c r="O159" s="17"/>
@@ -5213,7 +5243,7 @@
       <c r="I160" s="17"/>
       <c r="J160" s="18"/>
       <c r="K160" s="17"/>
-      <c r="L160" s="17"/>
+      <c r="L160" s="45"/>
       <c r="M160" s="18"/>
       <c r="N160" s="18"/>
       <c r="O160" s="17"/>
@@ -5238,7 +5268,7 @@
       <c r="I161" s="17"/>
       <c r="J161" s="18"/>
       <c r="K161" s="17"/>
-      <c r="L161" s="17"/>
+      <c r="L161" s="45"/>
       <c r="M161" s="18"/>
       <c r="N161" s="18"/>
       <c r="O161" s="17"/>
@@ -5263,7 +5293,7 @@
       <c r="I162" s="17"/>
       <c r="J162" s="18"/>
       <c r="K162" s="17"/>
-      <c r="L162" s="17"/>
+      <c r="L162" s="45"/>
       <c r="M162" s="18"/>
       <c r="N162" s="18"/>
       <c r="O162" s="17"/>
@@ -5288,7 +5318,7 @@
       <c r="I163" s="17"/>
       <c r="J163" s="18"/>
       <c r="K163" s="17"/>
-      <c r="L163" s="17"/>
+      <c r="L163" s="45"/>
       <c r="M163" s="18"/>
       <c r="N163" s="18"/>
       <c r="O163" s="17"/>
@@ -5313,7 +5343,7 @@
       <c r="I164" s="17"/>
       <c r="J164" s="18"/>
       <c r="K164" s="17"/>
-      <c r="L164" s="17"/>
+      <c r="L164" s="45"/>
       <c r="M164" s="18"/>
       <c r="N164" s="18"/>
       <c r="O164" s="17"/>
@@ -5338,7 +5368,7 @@
       <c r="I165" s="17"/>
       <c r="J165" s="18"/>
       <c r="K165" s="17"/>
-      <c r="L165" s="17"/>
+      <c r="L165" s="45"/>
       <c r="M165" s="18"/>
       <c r="N165" s="18"/>
       <c r="O165" s="17"/>
@@ -5363,7 +5393,7 @@
       <c r="I166" s="17"/>
       <c r="J166" s="18"/>
       <c r="K166" s="17"/>
-      <c r="L166" s="17"/>
+      <c r="L166" s="45"/>
       <c r="M166" s="18"/>
       <c r="N166" s="18"/>
       <c r="O166" s="17"/>
@@ -5388,7 +5418,7 @@
       <c r="I167" s="17"/>
       <c r="J167" s="18"/>
       <c r="K167" s="17"/>
-      <c r="L167" s="17"/>
+      <c r="L167" s="45"/>
       <c r="M167" s="18"/>
       <c r="N167" s="18"/>
       <c r="O167" s="17"/>
@@ -5413,7 +5443,7 @@
       <c r="I168" s="17"/>
       <c r="J168" s="18"/>
       <c r="K168" s="17"/>
-      <c r="L168" s="17"/>
+      <c r="L168" s="45"/>
       <c r="M168" s="18"/>
       <c r="N168" s="18"/>
       <c r="O168" s="17"/>
@@ -5438,7 +5468,7 @@
       <c r="I169" s="17"/>
       <c r="J169" s="18"/>
       <c r="K169" s="17"/>
-      <c r="L169" s="17"/>
+      <c r="L169" s="45"/>
       <c r="M169" s="18"/>
       <c r="N169" s="18"/>
       <c r="O169" s="17"/>
@@ -5463,7 +5493,7 @@
       <c r="I170" s="17"/>
       <c r="J170" s="18"/>
       <c r="K170" s="17"/>
-      <c r="L170" s="17"/>
+      <c r="L170" s="45"/>
       <c r="M170" s="18"/>
       <c r="N170" s="18"/>
       <c r="O170" s="17"/>
@@ -5488,7 +5518,7 @@
       <c r="I171" s="17"/>
       <c r="J171" s="18"/>
       <c r="K171" s="17"/>
-      <c r="L171" s="17"/>
+      <c r="L171" s="45"/>
       <c r="M171" s="18"/>
       <c r="N171" s="18"/>
       <c r="O171" s="17"/>
@@ -5513,7 +5543,7 @@
       <c r="I172" s="17"/>
       <c r="J172" s="18"/>
       <c r="K172" s="17"/>
-      <c r="L172" s="17"/>
+      <c r="L172" s="45"/>
       <c r="M172" s="18"/>
       <c r="N172" s="18"/>
       <c r="O172" s="17"/>
@@ -5538,7 +5568,7 @@
       <c r="I173" s="17"/>
       <c r="J173" s="18"/>
       <c r="K173" s="17"/>
-      <c r="L173" s="17"/>
+      <c r="L173" s="45"/>
       <c r="M173" s="18"/>
       <c r="N173" s="18"/>
       <c r="O173" s="17"/>
@@ -5563,7 +5593,7 @@
       <c r="I174" s="17"/>
       <c r="J174" s="18"/>
       <c r="K174" s="17"/>
-      <c r="L174" s="17"/>
+      <c r="L174" s="45"/>
       <c r="M174" s="18"/>
       <c r="N174" s="18"/>
       <c r="O174" s="17"/>
@@ -5588,7 +5618,7 @@
       <c r="I175" s="17"/>
       <c r="J175" s="18"/>
       <c r="K175" s="17"/>
-      <c r="L175" s="17"/>
+      <c r="L175" s="45"/>
       <c r="M175" s="18"/>
       <c r="N175" s="18"/>
       <c r="O175" s="17"/>
@@ -5613,7 +5643,7 @@
       <c r="I176" s="17"/>
       <c r="J176" s="18"/>
       <c r="K176" s="17"/>
-      <c r="L176" s="17"/>
+      <c r="L176" s="45"/>
       <c r="M176" s="18"/>
       <c r="N176" s="18"/>
       <c r="O176" s="17"/>
@@ -5638,7 +5668,7 @@
       <c r="I177" s="17"/>
       <c r="J177" s="18"/>
       <c r="K177" s="17"/>
-      <c r="L177" s="17"/>
+      <c r="L177" s="45"/>
       <c r="M177" s="18"/>
       <c r="N177" s="18"/>
       <c r="O177" s="17"/>
@@ -5663,7 +5693,7 @@
       <c r="I178" s="17"/>
       <c r="J178" s="18"/>
       <c r="K178" s="17"/>
-      <c r="L178" s="17"/>
+      <c r="L178" s="45"/>
       <c r="M178" s="18"/>
       <c r="N178" s="18"/>
       <c r="O178" s="17"/>
@@ -5688,7 +5718,7 @@
       <c r="I179" s="17"/>
       <c r="J179" s="18"/>
       <c r="K179" s="17"/>
-      <c r="L179" s="17"/>
+      <c r="L179" s="45"/>
       <c r="M179" s="18"/>
       <c r="N179" s="18"/>
       <c r="O179" s="17"/>
@@ -5713,7 +5743,7 @@
       <c r="I180" s="17"/>
       <c r="J180" s="18"/>
       <c r="K180" s="17"/>
-      <c r="L180" s="17"/>
+      <c r="L180" s="45"/>
       <c r="M180" s="18"/>
       <c r="N180" s="18"/>
       <c r="O180" s="17"/>
@@ -5738,7 +5768,7 @@
       <c r="I181" s="17"/>
       <c r="J181" s="18"/>
       <c r="K181" s="17"/>
-      <c r="L181" s="17"/>
+      <c r="L181" s="45"/>
       <c r="M181" s="18"/>
       <c r="N181" s="18"/>
       <c r="O181" s="17"/>
@@ -5763,7 +5793,7 @@
       <c r="I182" s="17"/>
       <c r="J182" s="18"/>
       <c r="K182" s="17"/>
-      <c r="L182" s="17"/>
+      <c r="L182" s="45"/>
       <c r="M182" s="18"/>
       <c r="N182" s="18"/>
       <c r="O182" s="17"/>
@@ -5788,7 +5818,7 @@
       <c r="I183" s="17"/>
       <c r="J183" s="18"/>
       <c r="K183" s="17"/>
-      <c r="L183" s="17"/>
+      <c r="L183" s="45"/>
       <c r="M183" s="18"/>
       <c r="N183" s="18"/>
       <c r="O183" s="17"/>
@@ -5813,7 +5843,7 @@
       <c r="I184" s="17"/>
       <c r="J184" s="18"/>
       <c r="K184" s="17"/>
-      <c r="L184" s="17"/>
+      <c r="L184" s="45"/>
       <c r="M184" s="18"/>
       <c r="N184" s="18"/>
       <c r="O184" s="17"/>
@@ -5838,7 +5868,7 @@
       <c r="I185" s="17"/>
       <c r="J185" s="18"/>
       <c r="K185" s="17"/>
-      <c r="L185" s="17"/>
+      <c r="L185" s="45"/>
       <c r="M185" s="18"/>
       <c r="N185" s="18"/>
       <c r="O185" s="17"/>
@@ -5863,7 +5893,7 @@
       <c r="I186" s="17"/>
       <c r="J186" s="18"/>
       <c r="K186" s="17"/>
-      <c r="L186" s="17"/>
+      <c r="L186" s="45"/>
       <c r="M186" s="18"/>
       <c r="N186" s="18"/>
       <c r="O186" s="17"/>
@@ -5888,7 +5918,7 @@
       <c r="I187" s="17"/>
       <c r="J187" s="18"/>
       <c r="K187" s="17"/>
-      <c r="L187" s="17"/>
+      <c r="L187" s="45"/>
       <c r="M187" s="18"/>
       <c r="N187" s="18"/>
       <c r="O187" s="17"/>
@@ -5913,7 +5943,7 @@
       <c r="I188" s="17"/>
       <c r="J188" s="18"/>
       <c r="K188" s="17"/>
-      <c r="L188" s="17"/>
+      <c r="L188" s="45"/>
       <c r="M188" s="18"/>
       <c r="N188" s="18"/>
       <c r="O188" s="17"/>
@@ -5938,7 +5968,7 @@
       <c r="I189" s="17"/>
       <c r="J189" s="18"/>
       <c r="K189" s="17"/>
-      <c r="L189" s="17"/>
+      <c r="L189" s="45"/>
       <c r="M189" s="18"/>
       <c r="N189" s="18"/>
       <c r="O189" s="17"/>
@@ -5963,7 +5993,7 @@
       <c r="I190" s="17"/>
       <c r="J190" s="18"/>
       <c r="K190" s="17"/>
-      <c r="L190" s="17"/>
+      <c r="L190" s="45"/>
       <c r="M190" s="18"/>
       <c r="N190" s="18"/>
       <c r="O190" s="17"/>
@@ -5988,7 +6018,7 @@
       <c r="I191" s="17"/>
       <c r="J191" s="18"/>
       <c r="K191" s="17"/>
-      <c r="L191" s="17"/>
+      <c r="L191" s="45"/>
       <c r="M191" s="18"/>
       <c r="N191" s="18"/>
       <c r="O191" s="17"/>
@@ -6013,7 +6043,7 @@
       <c r="I192" s="17"/>
       <c r="J192" s="18"/>
       <c r="K192" s="17"/>
-      <c r="L192" s="17"/>
+      <c r="L192" s="45"/>
       <c r="M192" s="18"/>
       <c r="N192" s="18"/>
       <c r="O192" s="17"/>
@@ -6038,7 +6068,7 @@
       <c r="I193" s="17"/>
       <c r="J193" s="18"/>
       <c r="K193" s="17"/>
-      <c r="L193" s="17"/>
+      <c r="L193" s="45"/>
       <c r="M193" s="18"/>
       <c r="N193" s="18"/>
       <c r="O193" s="17"/>
@@ -6063,7 +6093,7 @@
       <c r="I194" s="17"/>
       <c r="J194" s="18"/>
       <c r="K194" s="17"/>
-      <c r="L194" s="17"/>
+      <c r="L194" s="45"/>
       <c r="M194" s="18"/>
       <c r="N194" s="18"/>
       <c r="O194" s="17"/>
@@ -6088,7 +6118,7 @@
       <c r="I195" s="17"/>
       <c r="J195" s="18"/>
       <c r="K195" s="17"/>
-      <c r="L195" s="17"/>
+      <c r="L195" s="45"/>
       <c r="M195" s="18"/>
       <c r="N195" s="18"/>
       <c r="O195" s="17"/>
@@ -6113,7 +6143,7 @@
       <c r="I196" s="17"/>
       <c r="J196" s="18"/>
       <c r="K196" s="17"/>
-      <c r="L196" s="17"/>
+      <c r="L196" s="45"/>
       <c r="M196" s="18"/>
       <c r="N196" s="18"/>
       <c r="O196" s="17"/>
@@ -6138,7 +6168,7 @@
       <c r="I197" s="17"/>
       <c r="J197" s="18"/>
       <c r="K197" s="17"/>
-      <c r="L197" s="17"/>
+      <c r="L197" s="45"/>
       <c r="M197" s="18"/>
       <c r="N197" s="18"/>
       <c r="O197" s="17"/>
@@ -6163,7 +6193,7 @@
       <c r="I198" s="17"/>
       <c r="J198" s="18"/>
       <c r="K198" s="17"/>
-      <c r="L198" s="17"/>
+      <c r="L198" s="45"/>
       <c r="M198" s="18"/>
       <c r="N198" s="18"/>
       <c r="O198" s="17"/>
@@ -6188,7 +6218,7 @@
       <c r="I199" s="17"/>
       <c r="J199" s="18"/>
       <c r="K199" s="17"/>
-      <c r="L199" s="17"/>
+      <c r="L199" s="45"/>
       <c r="M199" s="18"/>
       <c r="N199" s="18"/>
       <c r="O199" s="17"/>
@@ -6213,7 +6243,7 @@
       <c r="I200" s="17"/>
       <c r="J200" s="18"/>
       <c r="K200" s="17"/>
-      <c r="L200" s="17"/>
+      <c r="L200" s="45"/>
       <c r="M200" s="18"/>
       <c r="N200" s="18"/>
       <c r="O200" s="17"/>
@@ -6238,7 +6268,7 @@
       <c r="I201" s="17"/>
       <c r="J201" s="18"/>
       <c r="K201" s="17"/>
-      <c r="L201" s="17"/>
+      <c r="L201" s="45"/>
       <c r="M201" s="18"/>
       <c r="N201" s="18"/>
       <c r="O201" s="17"/>
@@ -6263,7 +6293,7 @@
       <c r="I202" s="17"/>
       <c r="J202" s="18"/>
       <c r="K202" s="17"/>
-      <c r="L202" s="17"/>
+      <c r="L202" s="45"/>
       <c r="M202" s="18"/>
       <c r="N202" s="18"/>
       <c r="O202" s="17"/>
@@ -6288,7 +6318,7 @@
       <c r="I203" s="17"/>
       <c r="J203" s="18"/>
       <c r="K203" s="17"/>
-      <c r="L203" s="17"/>
+      <c r="L203" s="45"/>
       <c r="M203" s="18"/>
       <c r="N203" s="18"/>
       <c r="O203" s="17"/>
@@ -6313,7 +6343,7 @@
       <c r="I204" s="17"/>
       <c r="J204" s="18"/>
       <c r="K204" s="17"/>
-      <c r="L204" s="17"/>
+      <c r="L204" s="45"/>
       <c r="M204" s="18"/>
       <c r="N204" s="18"/>
       <c r="O204" s="17"/>
@@ -6338,7 +6368,7 @@
       <c r="I205" s="17"/>
       <c r="J205" s="18"/>
       <c r="K205" s="17"/>
-      <c r="L205" s="17"/>
+      <c r="L205" s="45"/>
       <c r="M205" s="18"/>
       <c r="N205" s="18"/>
       <c r="O205" s="17"/>
@@ -6363,7 +6393,7 @@
       <c r="I206" s="17"/>
       <c r="J206" s="18"/>
       <c r="K206" s="17"/>
-      <c r="L206" s="17"/>
+      <c r="L206" s="45"/>
       <c r="M206" s="18"/>
       <c r="N206" s="18"/>
       <c r="O206" s="17"/>

</xml_diff>

<commit_message>
For mercycorps/toladata#2548, tweak bulk import template.
</commit_message>
<xml_diff>
--- a/indicators/bulk_import_files/BulkIndicatorImportTemplate.xlsx
+++ b/indicators/bulk_import_files/BulkIndicatorImportTemplate.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sjogdeo/Sites/tolaActivity/TolaActivity/indicators/bulk_import_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE6391DC-6F14-224F-AA09-D10A541F8896}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2BDC0ED-F683-E145-A8CF-E2A0B544A743}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -797,7 +797,7 @@
   <dimension ref="A1:AJ933"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>

</xml_diff>